<commit_message>
backup shitcode of NCoMM
</commit_message>
<xml_diff>
--- a/2025国赛/result1.xlsx
+++ b/2025国赛/result1.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="问题三最优策略" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -16,17 +16,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+  </numFmts>
+  <fonts count="1">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -37,7 +36,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -45,21 +44,13 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -425,175 +416,210 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="40" customWidth="1" min="1" max="1"/>
+    <col width="20" customWidth="1" min="2" max="2"/>
+    <col width="20" customWidth="1" min="3" max="3"/>
+    <col width="20" customWidth="1" min="4" max="4"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>无人机编号</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>烟幕弹编号</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>飞行方向（度）</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>飞行速度（m/s）</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>投放点x</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>投放点y</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>投放点z</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>起爆点x</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>起爆点y</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>起爆点z</t>
+      <c r="A1" t="inlineStr"/>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>FY1</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>G1</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>179.4852</v>
-      </c>
-      <c r="D2" t="n">
-        <v>129.6711</v>
-      </c>
-      <c r="E2" t="n">
-        <v>17791.1527</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0.0795</v>
-      </c>
-      <c r="G2" t="n">
-        <v>1800</v>
-      </c>
-      <c r="H2" t="n">
-        <v>17319.8601</v>
-      </c>
-      <c r="I2" t="n">
-        <v>4.3144</v>
-      </c>
-      <c r="J2" t="n">
-        <v>1735.267</v>
+          <t>无人机运动方向</t>
+        </is>
+      </c>
+      <c r="B2" s="1" t="n">
+        <v>179.494932458148</v>
+      </c>
+      <c r="C2" s="1" t="n">
+        <v>179.494932458148</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>179.494932458148</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>FY1</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>G2</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>179.4852</v>
-      </c>
-      <c r="D3" t="n">
-        <v>129.6711</v>
-      </c>
-      <c r="E3" t="n">
-        <v>17587.0112</v>
-      </c>
-      <c r="F3" t="n">
-        <v>1.9139</v>
-      </c>
-      <c r="G3" t="n">
-        <v>1800</v>
-      </c>
-      <c r="H3" t="n">
-        <v>17000.5247</v>
-      </c>
-      <c r="I3" t="n">
-        <v>7.1838</v>
-      </c>
-      <c r="J3" t="n">
-        <v>1699.7555</v>
+          <t>无人机运动速度 (m/s)</t>
+        </is>
+      </c>
+      <c r="B3" s="1" t="n">
+        <v>137.7772949217882</v>
+      </c>
+      <c r="C3" s="1" t="n">
+        <v>137.7772949217882</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>137.7772949217882</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>FY1</t>
+          <t>烟幕干扰弹编号</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
+          <t>G1</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>G2</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
           <t>G3</t>
         </is>
       </c>
-      <c r="C4" t="n">
-        <v>179.4852</v>
-      </c>
-      <c r="D4" t="n">
-        <v>129.6711</v>
-      </c>
-      <c r="E4" t="n">
-        <v>17338.3036</v>
-      </c>
-      <c r="F4" t="n">
-        <v>4.1487</v>
-      </c>
-      <c r="G4" t="n">
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>烟幕干扰弹投放点的x坐标 (m)</t>
+        </is>
+      </c>
+      <c r="B5" s="1" t="n">
+        <v>17796.99761946272</v>
+      </c>
+      <c r="C5" s="1" t="n">
+        <v>17365.1100147684</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>16819.56695691718</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>烟幕干扰弹投放点的y坐标 (m)</t>
+        </is>
+      </c>
+      <c r="B6" s="1" t="n">
+        <v>0.02646694485384877</v>
+      </c>
+      <c r="C6" s="1" t="n">
+        <v>3.833694334772658</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>8.642830900989445</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>烟幕干扰弹投放点的z坐标 (m)</t>
+        </is>
+      </c>
+      <c r="B7" s="1" t="n">
         <v>1800</v>
       </c>
-      <c r="H4" t="n">
-        <v>16689.9742</v>
-      </c>
-      <c r="I4" t="n">
-        <v>9.974299999999999</v>
-      </c>
-      <c r="J4" t="n">
-        <v>1677.5</v>
+      <c r="C7" s="1" t="n">
+        <v>1800</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>烟幕干扰弹起爆点的x坐标 (m)</t>
+        </is>
+      </c>
+      <c r="B8" s="1" t="n">
+        <v>17284.23210549007</v>
+      </c>
+      <c r="C8" s="1" t="n">
+        <v>16676.41260114415</v>
+      </c>
+      <c r="D8" s="1" t="n">
+        <v>16301.09246219939</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>烟幕干扰弹起爆点的y坐标 (m)</t>
+        </is>
+      </c>
+      <c r="B9" s="1" t="n">
+        <v>4.54665897672333</v>
+      </c>
+      <c r="C9" s="1" t="n">
+        <v>9.9047823401168</v>
+      </c>
+      <c r="D9" s="1" t="n">
+        <v>13.21334942434694</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>烟幕干扰弹起爆点的z坐标 (m)</t>
+        </is>
+      </c>
+      <c r="B10" s="1" t="n">
+        <v>1732.124641198383</v>
+      </c>
+      <c r="C10" s="1" t="n">
+        <v>1677.55771539936</v>
+      </c>
+      <c r="D10" s="1" t="n">
+        <v>1730.60481875881</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>有效干扰时长 (s)</t>
+        </is>
+      </c>
+      <c r="B11" s="1" t="n">
+        <v>6.401780047052668</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>注：以x轴为正向，逆时针方向为正，取值0~360（度）。</t>
+        </is>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="A13:D13"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>